<commit_message>
Final daily scrum update, other doc work
</commit_message>
<xml_diff>
--- a/docs/deliverable2/Getana_Deliverable_2_DailyScrumReport.xlsx
+++ b/docs/deliverable2/Getana_Deliverable_2_DailyScrumReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45CCA66-96B4-DC49-BB82-DDB54274C517}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22791607-E962-9545-B8C3-D384ACDD49BD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="114">
   <si>
     <t>Daily Scrum Report — Sprint 1</t>
   </si>
@@ -311,12 +311,6 @@
     <t>What they have done: Completed work for saving/loading schedules</t>
   </si>
   <si>
-    <t xml:space="preserve">What they have done: Began working on map interface imlementation </t>
-  </si>
-  <si>
-    <t>What they will do: Update platform &amp; SRS/Use case model document. Create GRL &amp; UCM models document. Complete first app release implementation.</t>
-  </si>
-  <si>
     <t>What they will do:  Create GRL &amp; UCM models document. Complete first app release implementation.</t>
   </si>
   <si>
@@ -332,13 +326,49 @@
     <t>What they will do: Complete sprint 2 review , team member report, &amp; focus group document. Update sprint/product backlog at end of sprint. Complete first app release implementation. Create GRL &amp; UCM models document.</t>
   </si>
   <si>
-    <t>What they will do: Begin implementation tasks (Maps API code calls) assigned last Scrum meeting, Create configuration management plan document</t>
-  </si>
-  <si>
     <t>What they have done: Attended meeting, planned presentation</t>
   </si>
   <si>
     <t>What they will do: Implement driver code to utilize google maps API to generate route from provided schedule detail</t>
+  </si>
+  <si>
+    <t>What they have done: No work completed</t>
+  </si>
+  <si>
+    <t>What will they do: Not present for scrum meeting.</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Not present for scrum meeting.</t>
+  </si>
+  <si>
+    <t>What they have done: No work completed.</t>
+  </si>
+  <si>
+    <t>What they will do: Begin implementation tasks (Maps API code calls) assigned previously, Create configuration management plan document</t>
+  </si>
+  <si>
+    <t>What they will do: Enjoy spring break</t>
+  </si>
+  <si>
+    <t>What they have done: Completed first few user interface implementations</t>
+  </si>
+  <si>
+    <t>What they have done: Completed detailed design and domain model document, completed first few user interface implementations.</t>
+  </si>
+  <si>
+    <t>What they have done: Miscellaneous documentation tasks</t>
+  </si>
+  <si>
+    <t>What they have done: Completed first few user interface implementations, Miscellaneous implementation fixes, Implemented story number 4</t>
+  </si>
+  <si>
+    <t>What they will do: Update platform &amp; SRS/Use case model document. Created GRL &amp; UCM models document. Complete first app release implementation.</t>
+  </si>
+  <si>
+    <t>What they have done: Began working on map interface imlementation.</t>
+  </si>
+  <si>
+    <t>What they have done: Worked on GRL and UCM model document. Implemented showing route between start and destination points.</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView topLeftCell="A71" zoomScale="150" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -1681,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
@@ -1816,7 +1846,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C61" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
@@ -1944,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="137" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1986,12 +2016,12 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -2009,7 +2039,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -2027,7 +2057,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -2045,12 +2075,12 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
@@ -2063,12 +2093,12 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C25" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C26" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
@@ -2076,12 +2106,12 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.15">
@@ -2116,17 +2146,17 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C34" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C35" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.15">
@@ -2134,17 +2164,17 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C38" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C39" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.15">
@@ -2152,17 +2182,17 @@
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C42" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C43" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.15">
@@ -2170,17 +2200,17 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C46" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C47" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
@@ -2188,17 +2218,17 @@
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C50" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C51" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.15">
@@ -2206,17 +2236,17 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C54" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C55" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Moved file, doc work
</commit_message>
<xml_diff>
--- a/docs/deliverable2/Getana_Deliverable_2_DailyScrumReport.xlsx
+++ b/docs/deliverable2/Getana_Deliverable_2_DailyScrumReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC73CD6A-C98D-434B-A174-370B9DFE8A97}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8167419-B0C8-7F4A-B36A-B665BA66B31F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -320,9 +320,6 @@
     <t>What they will do: Update product backlog,Complete first app release implementation. Create domain model &amp; detailed design document.</t>
   </si>
   <si>
-    <t>What they will do:Create domain model &amp; detailed design document. Complete first app release implementation.</t>
-  </si>
-  <si>
     <t>What they will do: Complete sprint 2 review , team member report, &amp; focus group document. Update sprint/product backlog at end of sprint. Complete first app release implementation. Create GRL &amp; UCM models document.</t>
   </si>
   <si>
@@ -359,16 +356,19 @@
     <t>What they will do: Update platform &amp; SRS/Use case model document. Created GRL &amp; UCM models document. Complete first app release implementation.</t>
   </si>
   <si>
-    <t>What they have done: Began working on map interface imlementation.</t>
-  </si>
-  <si>
     <t>What they have done: Worked on GRL and UCM model document. Implemented showing route between start and destination points.</t>
   </si>
   <si>
-    <t>What they have done: Miscellaneous documentation tasks, Updated SRS and UML document</t>
-  </si>
-  <si>
-    <t>What they have done: Completed first few user interface implementations, Miscellaneous implementation fixes, Implemented story number 4, Updated SRS and UML document, Worked on GRL and UCM model document.</t>
+    <t>What they will do: Create domain model &amp; detailed design document. Complete first app release implementation.</t>
+  </si>
+  <si>
+    <t>What they have done: Began working on map interface implementation.</t>
+  </si>
+  <si>
+    <t>What they have done: Miscellaneous documentation tasks, Updated SRS and UML document, Created configuration management plan document.</t>
+  </si>
+  <si>
+    <t>What they have done: Completed first few user interface implementations, Miscellaneous implementation fixes, Implemented story number 4, Updated SRS and UML document, Worked on GRL and UCM model document. Created configuration management plan.</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
@@ -1846,7 +1846,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="137" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2016,12 +2016,12 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -2039,7 +2039,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -2057,7 +2057,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C17" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -2093,7 +2093,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
@@ -2106,7 +2106,7 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
@@ -2146,17 +2146,17 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.15">
@@ -2169,7 +2169,7 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.15">
@@ -2182,12 +2182,12 @@
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.15">
@@ -2200,12 +2200,12 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.15">
@@ -2223,7 +2223,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
@@ -2236,12 +2236,12 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>